<commit_message>
Lamashan post-kingdom-management and city
</commit_message>
<xml_diff>
--- a/Kingdom Management.xlsx
+++ b/Kingdom Management.xlsx
@@ -909,7 +909,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -954,15 +954,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1129,9 +1121,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1945080</xdr:colOff>
+      <xdr:colOff>1944720</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1145,7 +1137,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="9360"/>
-          <a:ext cx="8899560" cy="8219520"/>
+          <a:ext cx="8899560" cy="8219160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1159,16 +1151,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1009800</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1009800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>577080</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>113760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>666720</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1181,8 +1173,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3457800" y="5362560"/>
-          <a:ext cx="2036880" cy="1961640"/>
+          <a:off x="5495760" y="7324920"/>
+          <a:ext cx="2036160" cy="1961280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1203,9 +1195,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>18720</xdr:colOff>
+      <xdr:colOff>18360</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1218,8 +1210,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8773920" y="9360"/>
-          <a:ext cx="9005400" cy="8219520"/>
+          <a:off x="8774280" y="9360"/>
+          <a:ext cx="9006120" cy="8219160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1240,9 +1232,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1028160</xdr:colOff>
+      <xdr:colOff>1027800</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1255,8 +1247,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12328200" y="5362200"/>
-          <a:ext cx="2075400" cy="999720"/>
+          <a:off x="12329640" y="5362200"/>
+          <a:ext cx="2075040" cy="999360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1270,16 +1262,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>981000</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1047600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>703800</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>866160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>455760</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1789200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1292,8 +1284,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="2114280" y="5334120"/>
-          <a:ext cx="942480" cy="923400"/>
+          <a:off x="3057120" y="6257880"/>
+          <a:ext cx="942120" cy="923040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1314,9 +1306,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1085400</xdr:colOff>
+      <xdr:colOff>1085040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1713960</xdr:rowOff>
+      <xdr:rowOff>1713600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1330,7 +1322,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3438360" y="790560"/>
-          <a:ext cx="942480" cy="923400"/>
+          <a:ext cx="942120" cy="923040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1351,9 +1343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>990000</xdr:colOff>
+      <xdr:colOff>989640</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1704600</xdr:rowOff>
+      <xdr:rowOff>1704240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1366,8 +1358,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4532400" y="781200"/>
-          <a:ext cx="942480" cy="923400"/>
+          <a:off x="4533120" y="781200"/>
+          <a:ext cx="942120" cy="923040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1394,20 +1386,20 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.79"/>
   </cols>
   <sheetData>
@@ -1537,10 +1529,10 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="12" t="n">
+      <c r="B7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="9"/>
@@ -1548,19 +1540,17 @@
       <c r="E7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="12" t="n">
+      <c r="B8" s="11" t="n">
         <v>7</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="13"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
@@ -1568,10 +1558,8 @@
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="13"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -1641,7 +1629,7 @@
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="12" t="n">
+      <c r="B15" s="11" t="n">
         <v>6</v>
       </c>
       <c r="C15" s="7"/>
@@ -1690,13 +1678,13 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -1722,28 +1710,28 @@
       <c r="A20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="12" t="n">
+      <c r="C20" s="11" t="n">
         <v>5</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="18" t="n">
+      <c r="E20" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(E$19,$D20)),LEN(B20)&gt;0),$C20,0)</f>
         <v>5</v>
       </c>
-      <c r="F20" s="18" t="n">
+      <c r="F20" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(F$19,$D20)),LEN(B20)&gt;0),$C20,0)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="18" t="n">
+      <c r="G20" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(G$19,$D20)),D20&lt;&gt;""),$C20,0)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="19" t="n">
+      <c r="H20" s="17" t="n">
         <f aca="false">IF(LEN(B20)&gt;0,0,4)</f>
         <v>0</v>
       </c>
@@ -1756,28 +1744,28 @@
       <c r="A21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="12" t="n">
+      <c r="C21" s="11" t="n">
         <v>-1</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="18" t="n">
+      <c r="E21" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(E$19,$D21)),LEN(B21)&gt;0),$C21,0)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="18" t="n">
+      <c r="F21" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(F$19,$D21)),LEN(B21)&gt;0),$C21,0)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="18" t="n">
+      <c r="G21" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(G$19,$D21)),LEN(B21)&gt;0),$C21,0)</f>
         <v>-1</v>
       </c>
-      <c r="H21" s="19" t="n">
+      <c r="H21" s="17" t="n">
         <f aca="false">IF(LEN(B21)&gt;0,0,0)</f>
         <v>0</v>
       </c>
@@ -1790,26 +1778,26 @@
       <c r="A22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="12" t="n">
+      <c r="C22" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="18" t="n">
+      <c r="E22" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(F$19,$D22)),LEN(B22)&gt;0),$C22,IF(LEN(B22)=0,-2,0))</f>
         <v>3</v>
       </c>
-      <c r="G22" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="19" t="n">
+      <c r="G22" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="17" t="n">
         <f aca="false">IF(LEN(B22)&gt;0,0,1)</f>
         <v>0</v>
       </c>
@@ -1822,26 +1810,26 @@
       <c r="A23" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="12" t="n">
+      <c r="C23" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="18" t="n">
+      <c r="E23" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(G$19,$D23)),LEN(B23)&gt;0),$C23,IF(LEN(B23)=0,-4,0))</f>
         <v>4</v>
       </c>
-      <c r="H23" s="19" t="n">
+      <c r="H23" s="17" t="n">
         <f aca="false">IF(LEN(B23)&gt;0,0,0)</f>
         <v>0</v>
       </c>
@@ -1854,26 +1842,26 @@
       <c r="A24" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="12" t="n">
+      <c r="C24" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="18" t="n">
+      <c r="E24" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(G$19,$D24)),LEN(B24)&gt;0),$C24,IF(LEN(B24)=0,-2,0))</f>
         <v>5</v>
       </c>
-      <c r="H24" s="19" t="n">
+      <c r="H24" s="17" t="n">
         <f aca="false">IF(LEN(B24)&gt;0,0,0)</f>
         <v>0</v>
       </c>
@@ -1886,27 +1874,27 @@
       <c r="A25" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="12" t="n">
+      <c r="C25" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="19" t="n">
+      <c r="E25" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="17" t="n">
         <f aca="false">IF(LEN(B25)=0,-2,0)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="18" t="n">
+      <c r="G25" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(G$19,$D25)),LEN(B25)&gt;0),$C25,IF(LEN(B25)=0,-2,0))</f>
         <v>3</v>
       </c>
-      <c r="H25" s="19" t="n">
+      <c r="H25" s="17" t="n">
         <f aca="false">IF(LEN(B25)&gt;0,0,1)</f>
         <v>0</v>
       </c>
@@ -1919,26 +1907,26 @@
       <c r="A26" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="12" t="n">
+      <c r="C26" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="18" t="n">
+      <c r="E26" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(E$19,$D26)),LEN(B26)&gt;0),$C26,IF(B26="",-4,0))</f>
         <v>4</v>
       </c>
-      <c r="F26" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="19" t="n">
+      <c r="F26" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="17" t="n">
         <f aca="false">IF(LEN(B26)&gt;0,0,0)</f>
         <v>0</v>
       </c>
@@ -1951,26 +1939,26 @@
       <c r="A27" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="12" t="n">
+      <c r="C27" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="18" t="n">
+      <c r="E27" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(E$19,$D27)),LEN(B27)&gt;0),$C27,IF(B27="",-4,0))</f>
         <v>3</v>
       </c>
-      <c r="F27" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="19" t="n">
+      <c r="F27" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="17" t="n">
         <f aca="false">IF(LEN(B27)&gt;0,0,0)</f>
         <v>0</v>
       </c>
@@ -1983,26 +1971,26 @@
       <c r="A28" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="12" t="n">
+      <c r="C28" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="18" t="n">
+      <c r="E28" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(F$19,$D28)),LEN(B28)&gt;0),$C28,0)</f>
         <v>5</v>
       </c>
-      <c r="G28" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="19" t="n">
+      <c r="G28" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="17" t="n">
         <f aca="false">IF(LEN(B28)&gt;0,-1,0)</f>
         <v>-1</v>
       </c>
@@ -2015,28 +2003,28 @@
       <c r="A29" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="12" t="n">
+      <c r="C29" s="11" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="18" t="n">
+      <c r="E29" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(E$19,$D29)),LEN(B29)&gt;0),$C29,IF(B29="",-4,0))</f>
         <v>1</v>
       </c>
-      <c r="F29" s="18" t="n">
+      <c r="F29" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(F$19,$D29)),LEN(B29)&gt;0),$C29,0)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="18" t="n">
+      <c r="G29" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(G$19,$D29)),LEN(B29)&gt;0),$C29,0)</f>
         <v>0</v>
       </c>
-      <c r="H29" s="19" t="n">
+      <c r="H29" s="17" t="n">
         <f aca="false">IF(LEN(B29)&gt;0,0,1)</f>
         <v>0</v>
       </c>
@@ -2049,26 +2037,26 @@
       <c r="A30" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="12" t="n">
+      <c r="C30" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="18" t="n">
+      <c r="E30" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(E$19,$D30)),LEN(B30)&gt;0),$C30,IF(B30="",-4,0))</f>
         <v>5</v>
       </c>
-      <c r="F30" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="19" t="n">
+      <c r="F30" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="17" t="n">
         <f aca="false">IF(LEN(B30)&gt;0,0,0)</f>
         <v>0</v>
       </c>
@@ -2081,27 +2069,27 @@
       <c r="A31" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="12" t="n">
+      <c r="C31" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="18" t="n">
+      <c r="E31" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(F$19,$D31)),LEN(B31)&gt;0),$C31,IF(B31="",-4,0))</f>
         <v>4</v>
       </c>
-      <c r="G31" s="19" t="n">
+      <c r="G31" s="17" t="n">
         <f aca="false">IF(B31="",-2,0)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="19" t="n">
+      <c r="H31" s="17" t="n">
         <f aca="false">IF(LEN(B31)&gt;0,0,0)</f>
         <v>0</v>
       </c>
@@ -2111,22 +2099,22 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="21" t="n">
+      <c r="E32" s="19" t="n">
         <f aca="false">SUM(E20:E31)</f>
         <v>18</v>
       </c>
-      <c r="F32" s="21" t="n">
+      <c r="F32" s="19" t="n">
         <f aca="false">SUM(F20:F31)</f>
         <v>12</v>
       </c>
-      <c r="G32" s="21" t="n">
+      <c r="G32" s="19" t="n">
         <f aca="false">SUM(G20:G31)</f>
         <v>11</v>
       </c>
-      <c r="H32" s="21" t="n">
+      <c r="H32" s="19" t="n">
         <f aca="false">SUM(H20:H31)</f>
         <v>-1</v>
       </c>
@@ -2235,37 +2223,37 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="L6" s="20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2280,10 +2268,10 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="11"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
+      <c r="H7" s="9"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
@@ -2303,7 +2291,7 @@
       <c r="G8" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="11" t="n">
+      <c r="H8" s="9" t="n">
         <v>250</v>
       </c>
       <c r="J8" s="9" t="s">
@@ -2358,7 +2346,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="11" t="n">
+      <c r="G10" s="9" t="n">
         <v>3</v>
       </c>
       <c r="H10" s="9"/>
@@ -2673,171 +2661,171 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="Q1" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="R1" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="S1" s="24" t="s">
+      <c r="S1" s="22" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-    </row>
-    <row r="3" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+    </row>
+    <row r="3" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="26" t="n">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="24" t="n">
         <f aca="false">MAX(G5:G38)</f>
         <v>3</v>
       </c>
-      <c r="H3" s="26" t="n">
+      <c r="H3" s="24" t="n">
         <f aca="false">SUM(H5:H38)</f>
         <v>500</v>
       </c>
-      <c r="I3" s="26" t="n">
+      <c r="I3" s="24" t="n">
         <f aca="false">SUM(I5:I38)</f>
         <v>5</v>
       </c>
-      <c r="J3" s="26" t="n">
+      <c r="J3" s="24" t="n">
         <f aca="false">SUM(J5:J38)</f>
         <v>7</v>
       </c>
-      <c r="K3" s="26" t="n">
+      <c r="K3" s="24" t="n">
         <f aca="false">SUM(K5:K38)</f>
         <v>4</v>
       </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="26" t="n">
+      <c r="L3" s="9"/>
+      <c r="M3" s="24" t="n">
         <f aca="false">SUM(M5:M38)</f>
         <v>2</v>
       </c>
-      <c r="N3" s="26" t="n">
+      <c r="N3" s="24" t="n">
         <f aca="false">SUM(N5:N38)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="26" t="n">
+      <c r="O3" s="24" t="n">
         <f aca="false">SUM(O5:O38)</f>
         <v>0</v>
       </c>
-      <c r="P3" s="26" t="n">
+      <c r="P3" s="24" t="n">
         <f aca="false">SUM(P5:P38)</f>
         <v>8</v>
       </c>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-    </row>
-    <row r="4" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="12" t="s">
+      <c r="B5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>99</v>
       </c>
       <c r="E5" s="9" t="n">
@@ -2904,13 +2892,13 @@
       <c r="A6" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="12"/>
+      <c r="B6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="11"/>
       <c r="E6" s="9" t="n">
         <f aca="false">IF(AND(LEN($Q6)&gt;1,COUNTIF(A$5:A5,Q6)&gt;0), _xlfn.IFNA(VLOOKUP($A6,BuildingValues,2), "")/2, _xlfn.IFNA(VLOOKUP($A6,BuildingValues,2), ""))</f>
         <v>32</v>
@@ -2975,13 +2963,13 @@
       <c r="A7" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="B7" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>102</v>
       </c>
       <c r="E7" s="9" t="n">
@@ -3048,13 +3036,13 @@
       <c r="A8" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="B8" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>104</v>
       </c>
       <c r="E8" s="9" t="n">
@@ -3121,13 +3109,13 @@
       <c r="A9" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B9" s="12" t="n">
+      <c r="B9" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>106</v>
       </c>
       <c r="E9" s="9" t="n">
@@ -3194,13 +3182,13 @@
       <c r="A10" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="12" t="n">
+      <c r="B10" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="12"/>
+      <c r="C10" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11"/>
       <c r="E10" s="9" t="n">
         <f aca="false">IF(AND(LEN($Q10)&gt;1,COUNTIF(A$5:A9,Q10)&gt;0), _xlfn.IFNA(VLOOKUP($A10,BuildingValues,2), "")/2, _xlfn.IFNA(VLOOKUP($A10,BuildingValues,2), ""))</f>
         <v>3</v>
@@ -3263,13 +3251,13 @@
       <c r="A11" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="12" t="n">
+      <c r="B11" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="12"/>
+      <c r="C11" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="11"/>
       <c r="E11" s="9" t="n">
         <f aca="false">IF(AND(LEN($Q11)&gt;1,COUNTIF(A$5:A10,Q11)&gt;0), _xlfn.IFNA(VLOOKUP($A11,BuildingValues,2), "")/2, _xlfn.IFNA(VLOOKUP($A11,BuildingValues,2), ""))</f>
         <v>4</v>
@@ -3330,9 +3318,9 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -3351,9 +3339,9 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -3372,9 +3360,9 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A14,BuildingValues,2), "")</f>
         <v/>
@@ -3435,9 +3423,9 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A15,BuildingValues,2), "")</f>
         <v/>
@@ -3498,9 +3486,9 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A16,BuildingValues,2), "")</f>
         <v/>
@@ -3561,9 +3549,9 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A17,BuildingValues,2), "")</f>
         <v/>
@@ -3624,9 +3612,9 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A18,BuildingValues,2), "")</f>
         <v/>
@@ -3687,9 +3675,9 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A19,BuildingValues,2), "")</f>
         <v/>
@@ -3750,9 +3738,9 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A20,BuildingValues,2), "")</f>
         <v/>
@@ -3813,9 +3801,9 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A21,BuildingValues,2), "")</f>
         <v/>
@@ -3876,9 +3864,9 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A22,BuildingValues,2), "")</f>
         <v/>
@@ -3939,9 +3927,9 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
       <c r="E23" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A23,BuildingValues,2), "")</f>
         <v/>
@@ -4002,9 +3990,9 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A24,BuildingValues,2), "")</f>
         <v/>
@@ -4065,9 +4053,9 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A25,BuildingValues,2), "")</f>
         <v/>
@@ -4128,9 +4116,9 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A26,BuildingValues,2), "")</f>
         <v/>
@@ -4191,9 +4179,9 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
       <c r="E27" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A27,BuildingValues,2), "")</f>
         <v/>
@@ -4254,9 +4242,9 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
       <c r="E28" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A28,BuildingValues,2), "")</f>
         <v/>
@@ -4317,9 +4305,9 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
       <c r="E29" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A29,BuildingValues,2), "")</f>
         <v/>
@@ -4380,9 +4368,9 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A30,BuildingValues,2), "")</f>
         <v/>
@@ -4443,9 +4431,9 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A31,BuildingValues,2), "")</f>
         <v/>
@@ -4506,9 +4494,9 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A32,BuildingValues,2), "")</f>
         <v/>
@@ -4569,9 +4557,9 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A33,BuildingValues,2), "")</f>
         <v/>
@@ -4632,9 +4620,9 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A34,BuildingValues,2), "")</f>
         <v/>
@@ -4695,9 +4683,9 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
       <c r="E35" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A35,BuildingValues,2), "")</f>
         <v/>
@@ -4758,9 +4746,9 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
       <c r="E36" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A36,BuildingValues,2), "")</f>
         <v/>
@@ -4821,9 +4809,9 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A37,BuildingValues,2), "")</f>
         <v/>
@@ -4884,9 +4872,9 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
       <c r="E38" s="9" t="str">
         <f aca="false">_xlfn.IFNA(VLOOKUP($A38,BuildingValues,2), "")</f>
         <v/>
@@ -4982,40 +4970,40 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="21" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="7" t="n">
         <f aca="false">SUM(D4:D20)</f>
         <v>3</v>
@@ -5030,7 +5018,7 @@
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="11"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9"/>
@@ -5041,250 +5029,250 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
-      <c r="I3" s="11"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="12" t="n">
+      <c r="B4" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12" t="s">
+      <c r="B6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="12" t="n">
+      <c r="B7" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="B8" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="12" t="n">
+      <c r="B9" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12" t="n">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12" t="n">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5314,23 +5302,23 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="26" t="s">
         <v>125</v>
       </c>
     </row>
@@ -5592,7 +5580,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.58"/>
@@ -5612,96 +5600,96 @@
     <row r="5" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="29" t="s">
+      <c r="C55" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
-      <c r="J55" s="29"/>
-      <c r="K55" s="29"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="29"/>
-      <c r="N55" s="29"/>
-      <c r="O55" s="29"/>
-      <c r="P55" s="29"/>
-      <c r="Q55" s="29"/>
-      <c r="R55" s="29"/>
-      <c r="S55" s="29"/>
-      <c r="T55" s="29"/>
-      <c r="U55" s="29"/>
-      <c r="V55" s="29"/>
-      <c r="W55" s="29"/>
-      <c r="X55" s="29"/>
-      <c r="Y55" s="29"/>
-      <c r="Z55" s="29"/>
-      <c r="AA55" s="29"/>
-      <c r="AB55" s="29"/>
-      <c r="AC55" s="29"/>
-      <c r="AD55" s="29"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="27"/>
+      <c r="L55" s="27"/>
+      <c r="M55" s="27"/>
+      <c r="N55" s="27"/>
+      <c r="O55" s="27"/>
+      <c r="P55" s="27"/>
+      <c r="Q55" s="27"/>
+      <c r="R55" s="27"/>
+      <c r="S55" s="27"/>
+      <c r="T55" s="27"/>
+      <c r="U55" s="27"/>
+      <c r="V55" s="27"/>
+      <c r="W55" s="27"/>
+      <c r="X55" s="27"/>
+      <c r="Y55" s="27"/>
+      <c r="Z55" s="27"/>
+      <c r="AA55" s="27"/>
+      <c r="AB55" s="27"/>
+      <c r="AC55" s="27"/>
+      <c r="AD55" s="27"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="29"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="29"/>
-      <c r="I56" s="29"/>
-      <c r="J56" s="29"/>
-      <c r="K56" s="29"/>
-      <c r="L56" s="29"/>
-      <c r="M56" s="29"/>
-      <c r="N56" s="29"/>
-      <c r="O56" s="29"/>
-      <c r="P56" s="29"/>
-      <c r="Q56" s="29"/>
-      <c r="R56" s="29"/>
-      <c r="S56" s="29"/>
-      <c r="T56" s="29"/>
-      <c r="U56" s="29"/>
-      <c r="V56" s="29"/>
-      <c r="W56" s="29"/>
-      <c r="X56" s="29"/>
-      <c r="Y56" s="29"/>
-      <c r="Z56" s="29"/>
-      <c r="AA56" s="29"/>
-      <c r="AB56" s="29"/>
-      <c r="AC56" s="29"/>
-      <c r="AD56" s="29"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="27"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="27"/>
+      <c r="N56" s="27"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="27"/>
+      <c r="Q56" s="27"/>
+      <c r="R56" s="27"/>
+      <c r="S56" s="27"/>
+      <c r="T56" s="27"/>
+      <c r="U56" s="27"/>
+      <c r="V56" s="27"/>
+      <c r="W56" s="27"/>
+      <c r="X56" s="27"/>
+      <c r="Y56" s="27"/>
+      <c r="Z56" s="27"/>
+      <c r="AA56" s="27"/>
+      <c r="AB56" s="27"/>
+      <c r="AC56" s="27"/>
+      <c r="AD56" s="27"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="29"/>
-      <c r="D57" s="29"/>
-      <c r="E57" s="29"/>
-      <c r="F57" s="29"/>
-      <c r="G57" s="29"/>
-      <c r="H57" s="29"/>
-      <c r="I57" s="29"/>
-      <c r="J57" s="29"/>
-      <c r="K57" s="29"/>
-      <c r="L57" s="29"/>
-      <c r="M57" s="29"/>
-      <c r="N57" s="29"/>
-      <c r="O57" s="29"/>
-      <c r="P57" s="29"/>
-      <c r="Q57" s="29"/>
-      <c r="R57" s="29"/>
-      <c r="S57" s="29"/>
-      <c r="T57" s="29"/>
-      <c r="U57" s="29"/>
-      <c r="V57" s="29"/>
-      <c r="W57" s="29"/>
-      <c r="X57" s="29"/>
-      <c r="Y57" s="29"/>
-      <c r="Z57" s="29"/>
-      <c r="AA57" s="29"/>
-      <c r="AB57" s="29"/>
-      <c r="AC57" s="29"/>
-      <c r="AD57" s="29"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="27"/>
+      <c r="L57" s="27"/>
+      <c r="M57" s="27"/>
+      <c r="N57" s="27"/>
+      <c r="O57" s="27"/>
+      <c r="P57" s="27"/>
+      <c r="Q57" s="27"/>
+      <c r="R57" s="27"/>
+      <c r="S57" s="27"/>
+      <c r="T57" s="27"/>
+      <c r="U57" s="27"/>
+      <c r="V57" s="27"/>
+      <c r="W57" s="27"/>
+      <c r="X57" s="27"/>
+      <c r="Y57" s="27"/>
+      <c r="Z57" s="27"/>
+      <c r="AA57" s="27"/>
+      <c r="AB57" s="27"/>
+      <c r="AC57" s="27"/>
+      <c r="AD57" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5738,10 +5726,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5773,16 +5761,16 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="20" t="s">
         <v>153</v>
       </c>
     </row>
@@ -5978,25 +5966,25 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -6122,16 +6110,16 @@
       <c r="D10" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="32" t="s">
+      <c r="I14" s="30" t="s">
         <v>168</v>
       </c>
     </row>
@@ -6198,13 +6186,13 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="29" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6264,18 +6252,18 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="29" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="31" t="s">
         <v>169</v>
       </c>
       <c r="B33" s="9" t="n">
@@ -6284,7 +6272,7 @@
       <c r="C33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="33" t="n">
+      <c r="A34" s="31" t="n">
         <v>1</v>
       </c>
       <c r="B34" s="9" t="n">
@@ -6295,7 +6283,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="33" t="n">
+      <c r="A35" s="31" t="n">
         <v>6</v>
       </c>
       <c r="B35" s="9" t="n">
@@ -6306,7 +6294,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="33" t="n">
+      <c r="A36" s="31" t="n">
         <v>12</v>
       </c>
       <c r="B36" s="9" t="n">
@@ -6317,7 +6305,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="33" t="n">
+      <c r="A37" s="31" t="n">
         <v>24</v>
       </c>
       <c r="B37" s="9" t="n">
@@ -6328,49 +6316,49 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="C41" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="32" t="s">
+      <c r="D41" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="32" t="s">
+      <c r="E41" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F41" s="32" t="s">
+      <c r="F41" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="32" t="s">
+      <c r="G41" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="32" t="s">
+      <c r="H41" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="I41" s="32" t="s">
+      <c r="I41" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="J41" s="32" t="s">
+      <c r="J41" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="K41" s="32" t="s">
+      <c r="K41" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="L41" s="32" t="s">
+      <c r="L41" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="M41" s="32" t="s">
+      <c r="M41" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="N41" s="32" t="s">
+      <c r="N41" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="O41" s="32" t="s">
+      <c r="O41" s="30" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Jan 2021 / Calistra
</commit_message>
<xml_diff>
--- a/Kingdom Management.xlsx
+++ b/Kingdom Management.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="230">
   <si>
     <t xml:space="preserve">Kingdom Overview</t>
   </si>
@@ -155,321 +155,345 @@
     <t xml:space="preserve">Councilor</t>
   </si>
   <si>
+    <t xml:space="preserve">Eire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akiros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Diplomat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halungormm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Priest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marshal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chief Sootscale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Royal Assassin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alyssa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spymaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ewiggia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treasurer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deltoran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dalak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City Districts:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City Districts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Round</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berry Land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farm Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deltorans Folly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forest Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swamp Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kobalds Hex: Dragon Lair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mountain Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oleg’s Trading post</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grassland Farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bokken’s Hut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hillside Farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">River delta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City District</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adjacent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minor Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Major Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defence Modifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost Halved By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halves consumption </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halves  Loyalty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totals:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1bp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5c-6d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brothel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melianse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Werewolf/Murders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dragon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foreign Language Mutterings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travelling Gnome Issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grigori beheading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multicultural festival</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tygg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robe of Bones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feather Token Swan Boat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feather Token Whip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feather Token Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">piece of amber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple Silver Ring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A bit of bark from the Syth Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fey Bane Dwarven WarAxe (broken) +2/+2d6 against Fey</t>
+  </si>
+  <si>
     <t xml:space="preserve">Darsht</t>
   </si>
   <si>
-    <t xml:space="preserve">General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akiros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grand Diplomat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Halungormm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High Priest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magister</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Josef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marshal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chief Sootscale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Royal Assassin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alyssa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spymaster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oleg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treasurer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deltoran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dalak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City Districts:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Farms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bridge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City Districts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Round</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Berry Land</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Farm Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deltorans Folly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forest Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swamp Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kobalds Hex: Dragon Lair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mountain Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oleg’s Trading post</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grassland Farm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hillside Farm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Building</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City District</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adjacent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unrest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minor Items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medium Items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Major Items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defence Modifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost Halved By</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Halves consumption </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Halves  Loyalty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Totals:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1bp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Castle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5c-6d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">House</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brothel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Build Points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melianse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Werewolf/Murders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dragon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foreign Language Mutterings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travelling Gnome Issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grigori beheading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multicultural festival</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tygg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Worth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robe of Bones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1000G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feather Token Swan Boat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feather Token Whip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">500G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feather Token Tree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">piece of amber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simple Silver Ring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A bit of bark from the Syth Tree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fey Bane Dwarven WarAxe (broken) +2/+2d6 against Fey</t>
-  </si>
-  <si>
     <t xml:space="preserve">Magical Ring</t>
   </si>
   <si>
@@ -678,9 +702,6 @@
   </si>
   <si>
     <t xml:space="preserve">Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Piers</t>
   </si>
   <si>
     <t xml:space="preserve">Shrine</t>
@@ -1121,9 +1142,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1944720</xdr:colOff>
+      <xdr:colOff>1944000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1137,7 +1158,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="9360"/>
-          <a:ext cx="8899560" cy="8219160"/>
+          <a:ext cx="8899560" cy="8218440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1151,16 +1172,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>577080</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>595080</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>666720</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>261720</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1173,8 +1194,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="5495760" y="7324920"/>
-          <a:ext cx="2036160" cy="1961280"/>
+          <a:off x="9568800" y="11247840"/>
+          <a:ext cx="2035080" cy="1960560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1195,9 +1216,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>18360</xdr:colOff>
+      <xdr:colOff>17640</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1210,8 +1231,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8774280" y="9360"/>
-          <a:ext cx="9006120" cy="8219160"/>
+          <a:off x="8775000" y="9360"/>
+          <a:ext cx="9005400" cy="8218440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1232,9 +1253,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1027800</xdr:colOff>
+      <xdr:colOff>1027080</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1247,8 +1268,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12329640" y="5362200"/>
-          <a:ext cx="2075040" cy="999360"/>
+          <a:off x="12330000" y="5362200"/>
+          <a:ext cx="2074320" cy="998640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1262,16 +1283,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>703800</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>866160</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>147960</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>455760</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1789200</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1089720</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>14400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1284,8 +1305,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3057120" y="6257880"/>
-          <a:ext cx="942120" cy="923040"/>
+          <a:off x="4942080" y="8104320"/>
+          <a:ext cx="941760" cy="922320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1306,9 +1327,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1085040</xdr:colOff>
+      <xdr:colOff>1084320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1713600</xdr:rowOff>
+      <xdr:rowOff>1712880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1322,7 +1343,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3438360" y="790560"/>
-          <a:ext cx="942120" cy="923040"/>
+          <a:ext cx="941400" cy="922320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1343,9 +1364,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>989640</xdr:colOff>
+      <xdr:colOff>988920</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1704240</xdr:rowOff>
+      <xdr:rowOff>1703520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1358,8 +1379,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4533120" y="781200"/>
-          <a:ext cx="942120" cy="923040"/>
+          <a:off x="4533480" y="781200"/>
+          <a:ext cx="941400" cy="922320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1379,17 +1400,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.86"/>
@@ -1398,9 +1419,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1437,7 +1456,7 @@
       </c>
       <c r="H2" s="7" t="n">
         <f aca="false">Buildings!I3+C16+Events!D2+E32+C3+ROUNDDOWN('Kingdom Size'!D7/4, 0)-B7</f>
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I2" s="8" t="n">
         <f aca="false">ROUNDDOWN('Kingdom Size'!D7/4, 0)</f>
@@ -1468,7 +1487,7 @@
       </c>
       <c r="H3" s="7" t="n">
         <f aca="false">D3+D16+F32+Buildings!J3+Events!E2-B7</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" s="8"/>
     </row>
@@ -1478,7 +1497,7 @@
       </c>
       <c r="B4" s="7" t="n">
         <f aca="false">'Kingdom Size'!C2-1</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -1491,7 +1510,7 @@
       </c>
       <c r="H4" s="7" t="n">
         <f aca="false">E3+E16+G32+Buildings!K3+Events!F2+ROUNDDOWN('Kingdom Size'!D7/8, 0)-B7</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I4" s="8"/>
     </row>
@@ -1501,7 +1520,7 @@
       </c>
       <c r="B5" s="7" t="n">
         <f aca="false">20+B4</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1511,7 +1530,7 @@
       </c>
       <c r="H5" s="7" t="n">
         <f aca="false">B4+F16+'Kingdom Size'!C3+'Kingdom Size'!C1</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="I5" s="8"/>
     </row>
@@ -1521,7 +1540,7 @@
       </c>
       <c r="B6" s="7" t="n">
         <f aca="false">(250*B4)+'Kingdom Size'!C4</f>
-        <v>1500</v>
+        <v>2500</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -1544,7 +1563,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="11" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -1706,7 +1725,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
         <v>33</v>
       </c>
@@ -1714,14 +1733,14 @@
         <v>34</v>
       </c>
       <c r="C20" s="11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(E$19,$D20)),LEN(B20)&gt;0),$C20,0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F20" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(F$19,$D20)),LEN(B20)&gt;0),$C20,0)</f>
@@ -1740,7 +1759,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
         <v>33</v>
       </c>
@@ -1858,8 +1877,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="16" t="n">
-        <f aca="false">IF(AND(ISNUMBER(SEARCH(G$19,$D24)),LEN(B24)&gt;0),$C24,IF(LEN(B24)=0,-2,0))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H24" s="17" t="n">
         <f aca="false">IF(LEN(B24)&gt;0,0,0)</f>
@@ -1984,8 +2002,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="16" t="n">
-        <f aca="false">IF(AND(ISNUMBER(SEARCH(F$19,$D28)),LEN(B28)&gt;0),$C28,0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G28" s="17" t="n">
         <v>0</v>
@@ -1999,7 +2016,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
         <v>50</v>
       </c>
@@ -2007,14 +2024,14 @@
         <v>51</v>
       </c>
       <c r="C29" s="11" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(E$19,$D29)),LEN(B29)&gt;0),$C29,IF(B29="",-4,0))</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F29" s="16" t="n">
         <f aca="false">IF(AND(ISNUMBER(SEARCH(F$19,$D29)),LEN(B29)&gt;0),$C29,0)</f>
@@ -2033,7 +2050,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
         <v>52</v>
       </c>
@@ -2104,15 +2121,15 @@
       </c>
       <c r="E32" s="19" t="n">
         <f aca="false">SUM(E20:E31)</f>
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F32" s="19" t="n">
         <f aca="false">SUM(F20:F31)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G32" s="19" t="n">
         <f aca="false">SUM(G20:G31)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H32" s="19" t="n">
         <f aca="false">SUM(H20:H31)</f>
@@ -2161,29 +2178,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,7 +2204,7 @@
       </c>
       <c r="C1" s="7" t="n">
         <f aca="false">SUM(C8:C32)*-2</f>
-        <v>-8</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2201,7 +2213,7 @@
       </c>
       <c r="C2" s="7" t="n">
         <f aca="false">COUNTA(A8:A32)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2263,7 +2275,7 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="n">
         <f aca="false">SUM(D8:D32)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -2431,16 +2443,22 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="J14" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K14" s="9" t="n">
         <v>4</v>
@@ -2450,9 +2468,15 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+      <c r="A15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -2460,9 +2484,13 @@
       <c r="H15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9"/>
+      <c r="A16" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="C16" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -2470,11 +2498,19 @@
       <c r="H16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9"/>
+      <c r="A17" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="C17" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -2641,34 +2677,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="5" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>27</v>
@@ -2677,13 +2711,13 @@
         <v>66</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="G1" s="22" t="s">
         <v>64</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="I1" s="22" t="s">
         <v>3</v>
@@ -2695,28 +2729,28 @@
         <v>5</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="S1" s="22" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,7 +2776,7 @@
     </row>
     <row r="3" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -2751,15 +2785,15 @@
       <c r="F3" s="9"/>
       <c r="G3" s="24" t="n">
         <f aca="false">MAX(G5:G38)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H3" s="24" t="n">
         <f aca="false">SUM(H5:H38)</f>
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="I3" s="24" t="n">
         <f aca="false">SUM(I5:I38)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J3" s="24" t="n">
         <f aca="false">SUM(J5:J38)</f>
@@ -2767,7 +2801,7 @@
       </c>
       <c r="K3" s="24" t="n">
         <f aca="false">SUM(K5:K38)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L3" s="9"/>
       <c r="M3" s="24" t="n">
@@ -2792,13 +2826,13 @@
     </row>
     <row r="4" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -2817,7 +2851,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B5" s="11" t="n">
         <v>1</v>
@@ -2826,7 +2860,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E5" s="9" t="n">
         <f aca="false">IF(AND(LEN($Q5)&gt;1,COUNTIF(A4:A$5,Q5)&gt;0), _xlfn.IFNA(VLOOKUP($A5,BuildingValues,2), "")/2, _xlfn.IFNA(VLOOKUP($A5,BuildingValues,2), ""))</f>
@@ -2890,7 +2924,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B6" s="11" t="n">
         <v>1</v>
@@ -2961,7 +2995,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B7" s="11" t="n">
         <v>2</v>
@@ -2970,7 +3004,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E7" s="9" t="n">
         <f aca="false">IF(AND(LEN($Q7)&gt;1,COUNTIF(A$5:A6,Q7)&gt;0), _xlfn.IFNA(VLOOKUP($A7,BuildingValues,2), "")/2, _xlfn.IFNA(VLOOKUP($A7,BuildingValues,2), ""))</f>
@@ -3034,7 +3068,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B8" s="11" t="n">
         <v>2</v>
@@ -3043,7 +3077,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E8" s="9" t="n">
         <f aca="false">IF(AND(LEN($Q8)&gt;1,COUNTIF(A$5:A7,Q8)&gt;0), _xlfn.IFNA(VLOOKUP($A8,BuildingValues,2), "")/2, _xlfn.IFNA(VLOOKUP($A8,BuildingValues,2), ""))</f>
@@ -3107,7 +3141,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B9" s="11" t="n">
         <v>3</v>
@@ -3116,7 +3150,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E9" s="9" t="n">
         <f aca="false">IF(AND(LEN($Q9)&gt;1,COUNTIF(A$5:A7,Q9)&gt;0), _xlfn.IFNA(VLOOKUP($A9,BuildingValues,2), "")/2, _xlfn.IFNA(VLOOKUP($A9,BuildingValues,2), ""))</f>
@@ -3180,7 +3214,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B10" s="11" t="n">
         <v>4</v>
@@ -3249,7 +3283,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B11" s="11" t="n">
         <v>4</v>
@@ -3317,17 +3351,33 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+      <c r="A12" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="D12" s="11"/>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9" t="n">
+        <v>16</v>
+      </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="G12" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="H12" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I12" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+      <c r="K12" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
@@ -4951,7 +5001,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4961,23 +5011,21 @@
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>3</v>
@@ -4989,18 +5037,18 @@
         <v>5</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -5033,7 +5081,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B4" s="11" t="n">
         <v>2</v>
@@ -5049,12 +5097,12 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B5" s="11" t="n">
         <v>4</v>
@@ -5070,12 +5118,12 @@
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B6" s="11" t="n">
         <v>1</v>
@@ -5087,12 +5135,12 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B7" s="11" t="n">
         <v>3</v>
@@ -5104,12 +5152,12 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B8" s="11" t="n">
         <v>2</v>
@@ -5124,7 +5172,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B9" s="11" t="n">
         <v>5</v>
@@ -5140,12 +5188,12 @@
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -5157,12 +5205,12 @@
         <v>4</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -5289,7 +5337,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5299,66 +5347,63 @@
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>65</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9"/>
       <c r="B2" s="9" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="D3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
       <c r="B4" s="9" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="D4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9"/>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D5" s="9"/>
     </row>
@@ -5367,37 +5412,37 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="D7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9"/>
       <c r="B9" s="9" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C9" s="9" t="n">
         <v>0</v>
@@ -5407,17 +5452,17 @@
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -5425,7 +5470,7 @@
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
       <c r="B12" s="9" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -5433,7 +5478,7 @@
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
@@ -5566,7 +5611,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5576,7 +5621,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.29"/>
@@ -5590,7 +5635,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="138.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5601,7 +5645,7 @@
     <row r="6" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="27" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D55" s="27"/>
       <c r="E55" s="27"/>
@@ -5707,7 +5751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5717,25 +5761,23 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="28" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="9" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C2" s="9" t="n">
         <f aca="false">Buildings!M3</f>
@@ -5744,7 +5786,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="9" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C3" s="9" t="n">
         <f aca="false">Buildings!N3</f>
@@ -5753,7 +5795,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="9" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="C4" s="9" t="n">
         <f aca="false">Buildings!O3</f>
@@ -5765,13 +5807,13 @@
         <v>64</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5779,7 +5821,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -5789,7 +5831,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -5944,7 +5986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5954,26 +5996,23 @@
       <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>3</v>
@@ -5990,7 +6029,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B2" s="9" t="n">
         <v>2</v>
@@ -6005,7 +6044,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9" t="n">
@@ -6020,7 +6059,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="n">
@@ -6043,12 +6082,12 @@
         <v>2</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -6056,12 +6095,12 @@
         <v>4</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="n">
@@ -6069,12 +6108,12 @@
       </c>
       <c r="D7" s="9"/>
       <c r="I7" s="9" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B8" s="9" t="n">
         <v>4</v>
@@ -6082,12 +6121,12 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="I8" s="9" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B9" s="9" t="n">
         <v>2</v>
@@ -6099,7 +6138,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B10" s="9" t="n">
         <v>2</v>
@@ -6111,7 +6150,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>5</v>
@@ -6120,24 +6159,24 @@
         <v>19</v>
       </c>
       <c r="I14" s="30" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B15" s="9" t="n">
         <v>-1</v>
       </c>
       <c r="C15" s="9"/>
       <c r="I15" s="9" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B16" s="9" t="n">
         <v>1</v>
@@ -6146,7 +6185,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6160,12 +6199,12 @@
         <v>2</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B18" s="9" t="n">
         <v>3</v>
@@ -6176,7 +6215,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B19" s="9" t="n">
         <v>4</v>
@@ -6187,7 +6226,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="29" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>3</v>
@@ -6198,7 +6237,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B24" s="9" t="n">
         <v>0</v>
@@ -6209,7 +6248,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B25" s="9" t="n">
         <v>1</v>
@@ -6231,7 +6270,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B27" s="9" t="n">
         <v>3</v>
@@ -6242,7 +6281,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B28" s="9" t="n">
         <v>4</v>
@@ -6253,7 +6292,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B32" s="29" t="s">
         <v>4</v>
@@ -6264,7 +6303,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="31" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B33" s="9" t="n">
         <v>-1</v>
@@ -6317,16 +6356,16 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="30" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B41" s="30" t="s">
         <v>66</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E41" s="30" t="s">
         <v>3</v>
@@ -6338,33 +6377,33 @@
         <v>5</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="I41" s="30" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="J41" s="30" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="K41" s="30" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="L41" s="30" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="M41" s="30" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="N41" s="30" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="O41" s="30" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B42" s="9" t="n">
         <v>52</v>
@@ -6388,20 +6427,20 @@
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
       <c r="M42" s="9" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B43" s="9" t="n">
         <v>18</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D43" s="9" t="n">
         <v>1000</v>
@@ -6424,7 +6463,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B44" s="9" t="n">
         <v>40</v>
@@ -6443,13 +6482,13 @@
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="N44" s="9" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="O44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B45" s="9" t="n">
         <v>12</v>
@@ -6469,20 +6508,20 @@
         <v>2</v>
       </c>
       <c r="M45" s="9" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B46" s="9" t="n">
         <v>50</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D46" s="9" t="n">
         <v>2000</v>
@@ -6508,14 +6547,14 @@
       </c>
       <c r="L46" s="9"/>
       <c r="M46" s="9" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B47" s="9" t="n">
         <v>6</v>
@@ -6540,13 +6579,13 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B48" s="9" t="n">
         <v>4</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9" t="n">
@@ -6564,14 +6603,14 @@
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
       <c r="M48" s="9" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="N48" s="9"/>
       <c r="O48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B49" s="9" t="n">
         <v>30</v>
@@ -6595,14 +6634,14 @@
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
       <c r="M49" s="9" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="N49" s="9"/>
       <c r="O49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B50" s="9" t="n">
         <v>54</v>
@@ -6633,7 +6672,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B51" s="9" t="n">
         <v>58</v>
@@ -6658,13 +6697,13 @@
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
       <c r="N51" s="9" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="O51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B52" s="9" t="n">
         <v>8</v>
@@ -6684,14 +6723,14 @@
         <v>4</v>
       </c>
       <c r="M52" s="9" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B53" s="9" t="n">
         <v>4</v>
@@ -6711,20 +6750,20 @@
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
       <c r="M53" s="9" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B54" s="9" t="n">
         <v>10</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
@@ -6742,14 +6781,14 @@
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B55" s="9" t="n">
         <v>28</v>
@@ -6771,14 +6810,14 @@
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B56" s="9" t="n">
         <v>12</v>
@@ -6798,14 +6837,14 @@
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
       <c r="M56" s="9" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B57" s="9" t="n">
         <v>4</v>
@@ -6825,20 +6864,20 @@
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
       <c r="M57" s="9" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B58" s="9" t="n">
         <v>34</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D58" s="9" t="n">
         <v>1000</v>
@@ -6856,20 +6895,20 @@
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
       <c r="M58" s="9" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B59" s="9" t="n">
         <v>10</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
@@ -6892,7 +6931,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B60" s="9" t="n">
         <v>3</v>
@@ -6915,13 +6954,13 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B61" s="9" t="n">
         <v>10</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D61" s="9" t="n">
         <v>500</v>
@@ -6939,14 +6978,14 @@
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
       <c r="M61" s="9" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="N61" s="9"/>
       <c r="O61" s="9"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B62" s="9" t="n">
         <v>14</v>
@@ -6968,14 +7007,14 @@
       <c r="K62" s="9"/>
       <c r="L62" s="9"/>
       <c r="M62" s="9" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="N62" s="9"/>
       <c r="O62" s="9"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B63" s="9" t="n">
         <v>6</v>
@@ -6995,20 +7034,20 @@
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
       <c r="M63" s="9" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="N63" s="9"/>
       <c r="O63" s="9"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B64" s="9" t="n">
         <v>28</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D64" s="9" t="n">
         <v>2000</v>
@@ -7026,20 +7065,20 @@
       <c r="K64" s="9"/>
       <c r="L64" s="9"/>
       <c r="M64" s="9" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="N64" s="9"/>
       <c r="O64" s="9"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B65" s="9" t="n">
         <v>68</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D65" s="9" t="n">
         <v>2000</v>
@@ -7061,14 +7100,14 @@
       </c>
       <c r="L65" s="9"/>
       <c r="M65" s="9" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="N65" s="9"/>
       <c r="O65" s="9"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="B66" s="9" t="n">
         <v>10</v>
@@ -7086,20 +7125,20 @@
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
       <c r="M66" s="9" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="N66" s="9"/>
       <c r="O66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B67" s="9" t="n">
         <v>48</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D67" s="9" t="n">
         <v>2000</v>
@@ -7119,20 +7158,20 @@
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
       <c r="M67" s="9" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="N67" s="9"/>
       <c r="O67" s="9"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="B68" s="9" t="n">
         <v>6</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="9" t="n">
@@ -7153,7 +7192,7 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B69" s="9" t="n">
         <v>6</v>
@@ -7173,14 +7212,14 @@
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
       <c r="M69" s="9" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="N69" s="9"/>
       <c r="O69" s="9"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B70" s="9" t="n">
         <v>24</v>
@@ -7202,14 +7241,14 @@
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
       <c r="M70" s="9" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="N70" s="9"/>
       <c r="O70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="9" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B71" s="9" t="n">
         <v>4</v>
@@ -7229,20 +7268,20 @@
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
       <c r="M71" s="9" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="N71" s="9"/>
       <c r="O71" s="9"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9" t="s">
-        <v>212</v>
+        <v>114</v>
       </c>
       <c r="B72" s="9" t="n">
         <v>16</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="D72" s="9" t="n">
         <v>1000</v>
@@ -7260,20 +7299,20 @@
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
       <c r="M72" s="9" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="N72" s="9"/>
       <c r="O72" s="9"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="9" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B73" s="9" t="n">
         <v>8</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D73" s="9" t="n">
         <v>500</v>
@@ -7289,14 +7328,14 @@
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="N73" s="9"/>
       <c r="O73" s="9"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="B74" s="9" t="n">
         <v>8</v>
@@ -7318,14 +7357,14 @@
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="N74" s="9"/>
       <c r="O74" s="9"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="B75" s="9" t="n">
         <v>6</v>
@@ -7350,13 +7389,13 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="B76" s="9" t="n">
         <v>10</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D76" s="9" t="n">
         <v>500</v>
@@ -7374,20 +7413,20 @@
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
       <c r="M76" s="9" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="N76" s="9"/>
       <c r="O76" s="9"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="B77" s="9" t="n">
         <v>6</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="D77" s="9"/>
       <c r="E77" s="9" t="n">
@@ -7408,13 +7447,13 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="9" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="B78" s="9" t="n">
         <v>12</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D78" s="9" t="n">
         <v>500</v>
@@ -7432,14 +7471,14 @@
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
       <c r="M78" s="9" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="N78" s="9"/>
       <c r="O78" s="9"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B79" s="9" t="n">
         <v>32</v>
@@ -7463,14 +7502,14 @@
       <c r="K79" s="9"/>
       <c r="L79" s="9"/>
       <c r="M79" s="9" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="N79" s="9"/>
       <c r="O79" s="9"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B80" s="9" t="n">
         <v>1</v>
@@ -7493,7 +7532,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B81" s="9" t="n">
         <v>24</v>
@@ -7513,14 +7552,14 @@
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
       <c r="M81" s="9" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="N81" s="9"/>
       <c r="O81" s="9"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="9" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B82" s="9" t="n">
         <v>22</v>
@@ -7542,20 +7581,20 @@
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
       <c r="M82" s="9" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="N82" s="9"/>
       <c r="O82" s="9"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="9" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="B83" s="9" t="n">
         <v>10</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D83" s="9" t="n">
         <v>500</v>
@@ -7573,14 +7612,14 @@
       <c r="K83" s="9"/>
       <c r="L83" s="9"/>
       <c r="M83" s="9" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="N83" s="9"/>
       <c r="O83" s="9"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="B84" s="9" t="n">
         <v>6</v>
@@ -7602,20 +7641,20 @@
         <v>2</v>
       </c>
       <c r="M84" s="9" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="N84" s="9"/>
       <c r="O84" s="9"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B85" s="9" t="n">
         <v>90</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="D85" s="9" t="n">
         <v>4000</v>
@@ -7639,7 +7678,7 @@
       <c r="M85" s="9"/>
       <c r="N85" s="9"/>
       <c r="O85" s="9" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>